<commit_message>
add edge case for import
</commit_message>
<xml_diff>
--- a/tests/integration/stubs/terminplan-v1.xlsx
+++ b/tests/integration/stubs/terminplan-v1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F8D1C5-956A-4E3B-BF45-09C7A3DE689A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7D1CAE-5FCC-44A9-96E6-B6A63656D416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termine" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>KW</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>Nachbefragung in Klassenstunde: GYM3 Klassen</t>
-  </si>
-  <si>
-    <t>01.03.2024</t>
   </si>
   <si>
     <t>QE führt die Klassenstunde mit den einsprachigen Klassen des JG. 25 durch</t>
@@ -593,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -683,7 +680,7 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y1" t="s">
         <v>23</v>
@@ -715,7 +712,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
@@ -779,20 +776,20 @@
       <c r="D3" s="3">
         <v>45348</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45353</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
@@ -831,13 +828,13 @@
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W3" t="s">
         <v>31</v>
       </c>
       <c r="X3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y3" t="s">
         <v>29</v>
@@ -848,28 +845,28 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2">
         <v>0.51041666666666663</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2">
         <v>0.57291666666666663</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" t="s">
         <v>29</v>
@@ -893,13 +890,13 @@
         <v>1</v>
       </c>
       <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="s">
         <v>46</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>47</v>
-      </c>
-      <c r="X4" t="s">
-        <v>48</v>
       </c>
       <c r="Y4" t="s">
         <v>29</v>
@@ -913,7 +910,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3">
         <v>45432</v>
@@ -922,13 +919,13 @@
         <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -970,7 +967,7 @@
         <v>29</v>
       </c>
       <c r="W5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X5" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
use new import format
</commit_message>
<xml_diff>
--- a/tests/integration/stubs/terminplan-v1.xlsx
+++ b/tests/integration/stubs/terminplan-v1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7D1CAE-5FCC-44A9-96E6-B6A63656D416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F054AA-C9DE-4590-904E-4AD10D5E8142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termine" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="58">
   <si>
     <t>KW</t>
   </si>
@@ -44,18 +44,6 @@
     <t>Beschreibung</t>
   </si>
   <si>
-    <t>GBSL</t>
-  </si>
-  <si>
-    <t>GBSL/GBJB</t>
-  </si>
-  <si>
-    <t>GBJB</t>
-  </si>
-  <si>
-    <t>GBJB/GBSL</t>
-  </si>
-  <si>
     <t>FMS</t>
   </si>
   <si>
@@ -171,6 +159,36 @@
   </si>
   <si>
     <t>Pfingstmontag: Frei</t>
+  </si>
+  <si>
+    <t>GYMD</t>
+  </si>
+  <si>
+    <t>GYMD/GYMF</t>
+  </si>
+  <si>
+    <t>GYMF</t>
+  </si>
+  <si>
+    <t>GYMF/GYMD</t>
+  </si>
+  <si>
+    <t>FMS/ECG</t>
+  </si>
+  <si>
+    <t>Di</t>
+  </si>
+  <si>
+    <t>Singen</t>
+  </si>
+  <si>
+    <t>Gemeinsam singen</t>
+  </si>
+  <si>
+    <t>Ausgeschlossene Klassen</t>
+  </si>
+  <si>
+    <t>25Ga, 25Gh</t>
   </si>
 </sst>
 </file>
@@ -233,9 +251,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Termine" displayName="Termine" ref="A1:Y5">
-  <autoFilter ref="A1:Y5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Termine" displayName="Termine" ref="A1:AA5">
+  <autoFilter ref="A1:AA5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="KW" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Wochentag"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Titel"/>
@@ -245,11 +263,12 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Zeit Ende"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ort"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Beschreibung"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="GBSL"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GBSL/GBJB"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="GBJB"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GBJB/GBSL"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="FMS"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="GYMD"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GYMD/GYMF"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="GYMF"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GYMF/GYMD"/>
+    <tableColumn id="26" xr3:uid="{AB31367F-7F4F-490E-93DB-986C98637B13}" name="FMS"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="FMS/ECG"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="ECG"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="ECG/FMS"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="WMS"/>
@@ -258,6 +277,7 @@
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Passerelle"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Bilingue LP's betroffen"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Klassen"/>
+    <tableColumn id="27" xr3:uid="{374E107A-BD74-4BF1-93B5-33E875F2FB7B}" name="Ausgeschlossene Klassen"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Betrifft"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Unterricht Betroffen?"/>
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Gelöscht Am"/>
@@ -588,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -604,12 +624,16 @@
     <col min="6" max="6" width="15" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="7" max="7" width="12" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="8" max="9" width="20" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="10" max="20" width="4" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="22" max="24" width="10" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="25" max="25" width="15" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="10" max="13" width="4" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="14" max="14" width="4" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="21" width="4" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="23" max="23" width="10" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="24" max="24" width="10" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="26" width="10" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="27" max="27" width="15" customWidth="1" outlineLevel="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="65" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,140 +662,146 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="Z2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="AA2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W2" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3">
         <v>45348</v>
@@ -786,146 +816,146 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3">
+        <v>25</v>
+      </c>
+      <c r="U3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3">
         <v>0</v>
       </c>
-      <c r="V3" t="s">
-        <v>36</v>
-      </c>
       <c r="W3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="Y3" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>0.51041666666666663</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2">
         <v>0.57291666666666663</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>25</v>
       </c>
       <c r="S4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="T4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4">
+        <v>25</v>
+      </c>
+      <c r="U4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4">
         <v>1</v>
       </c>
-      <c r="V4" t="s">
-        <v>45</v>
-      </c>
       <c r="W4" t="s">
-        <v>46</v>
-      </c>
-      <c r="X4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="Y4" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3">
         <v>45432</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -934,46 +964,111 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
-        <v>29</v>
-      </c>
       <c r="P5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5">
+        <v>25</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5">
         <v>1</v>
       </c>
-      <c r="R5" t="s">
-        <v>29</v>
-      </c>
       <c r="S5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="T5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U5">
+        <v>25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5">
         <v>0</v>
       </c>
-      <c r="V5" t="s">
-        <v>29</v>
-      </c>
       <c r="W5" t="s">
-        <v>39</v>
-      </c>
-      <c r="X5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Y5" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45433</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>45433</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" t="s">
+        <v>25</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>